<commit_message>
Updated demo's to be a better comparison, added new way to populate data
</commit_message>
<xml_diff>
--- a/FastExcelDemo/Template.xlsx
+++ b/FastExcelDemo/Template.xlsx
@@ -10,6 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -424,4 +425,18 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>